<commit_message>
Update Maps and Table Ref Document for PowerCube Detector Input
</commit_message>
<xml_diff>
--- a/bin/org/usfirst/frc/team1322/robot/RefDocs/FRC1322_ProgTeam_MapAndTables.xlsx
+++ b/bin/org/usfirst/frc/team1322/robot/RefDocs/FRC1322_ProgTeam_MapAndTables.xlsx
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="27">
-  <si>
-    <t>Motor List</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="34">
   <si>
     <t>IDs</t>
   </si>
@@ -35,83 +32,107 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Same Direction</t>
-  </si>
-  <si>
-    <t>0,1</t>
-  </si>
-  <si>
-    <t>2,3</t>
-  </si>
-  <si>
-    <t>4,5</t>
-  </si>
-  <si>
-    <t>6,7</t>
-  </si>
-  <si>
-    <t>8,9</t>
-  </si>
-  <si>
     <t>R Claw</t>
   </si>
   <si>
     <t>L Claw</t>
   </si>
   <si>
-    <t>Lift</t>
-  </si>
-  <si>
-    <t>RR Mechanem</t>
-  </si>
-  <si>
-    <t>RF Mechanem</t>
-  </si>
-  <si>
-    <t>LR Mechanem</t>
-  </si>
-  <si>
-    <t>LF Mechanem</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>Pneumatic Controls</t>
-  </si>
-  <si>
-    <t>Sensor List</t>
-  </si>
-  <si>
-    <t>*not used*</t>
-  </si>
-  <si>
-    <t>Lift Shifter</t>
-  </si>
-  <si>
-    <t>Claw</t>
-  </si>
-  <si>
-    <t>Analog or Digital</t>
-  </si>
-  <si>
     <t>I/O Mapping</t>
   </si>
   <si>
-    <t>Claw Lift</t>
+    <t>LIFT_SHIFT_O</t>
+  </si>
+  <si>
+    <t>LIFT_SHIFT_C</t>
+  </si>
+  <si>
+    <t>CLAW_CLOSE_O</t>
+  </si>
+  <si>
+    <t>CLAW_CLOSE_C</t>
+  </si>
+  <si>
+    <t>CLAW_LIFT_O</t>
+  </si>
+  <si>
+    <t>CLAW_LIFT_C</t>
+  </si>
+  <si>
+    <t>RR_MECH_1</t>
+  </si>
+  <si>
+    <t>RR_MECH_2</t>
+  </si>
+  <si>
+    <t>RF_MECH_1</t>
+  </si>
+  <si>
+    <t>RF_MECH_2</t>
+  </si>
+  <si>
+    <t>LR_MECH_1</t>
+  </si>
+  <si>
+    <t>LR_MECH_2</t>
+  </si>
+  <si>
+    <t>LF_MECH_1</t>
+  </si>
+  <si>
+    <t>LF_MECH_2</t>
+  </si>
+  <si>
+    <t>LIFT_1</t>
+  </si>
+  <si>
+    <t>LIFT_2</t>
+  </si>
+  <si>
+    <t>USB Controllers</t>
+  </si>
+  <si>
+    <t>USB_Driver</t>
+  </si>
+  <si>
+    <t>USB_AUX</t>
+  </si>
+  <si>
+    <t>COMPRESSOR</t>
+  </si>
+  <si>
+    <t>Motor Drivers</t>
+  </si>
+  <si>
+    <t>Binary Drivers</t>
+  </si>
+  <si>
+    <t>*do not use*</t>
+  </si>
+  <si>
+    <t>Pneumatic Drivers</t>
+  </si>
+  <si>
+    <t>Analog Sensor Inputs</t>
+  </si>
+  <si>
+    <t>Digital Sensor Inputs</t>
+  </si>
+  <si>
+    <t>Speed/PWM Inputs</t>
+  </si>
+  <si>
+    <t>TBD</t>
+  </si>
+  <si>
+    <t>PowerCube Detector</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,6 +164,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -152,7 +186,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -343,11 +377,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -371,9 +431,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -396,12 +453,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -716,259 +782,585 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
-    <col min="3" max="3" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="26.42578125" customWidth="1"/>
+    <col min="3" max="3" width="14" customWidth="1"/>
     <col min="4" max="4" width="12.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="19" t="s">
+    <row r="1" spans="1:2" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="A1" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="14" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" ht="31.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="15" t="s">
+      <c r="B4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="16" t="s">
+    </row>
+    <row r="5" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8">
+        <v>0</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="8">
+        <v>1</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
         <v>2</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="B7" s="9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
         <v>3</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="B8" s="9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="8" t="s">
+      <c r="B9" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
         <v>5</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="9">
+      <c r="B10" s="9" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>6</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>7</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>8</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>9</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>11</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C20" s="10"/>
+      <c r="D20" s="11"/>
+    </row>
+    <row r="21" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
+        <v>0</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="10"/>
+      <c r="D21" s="12"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>1</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="10"/>
+      <c r="D22" s="12"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>2</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3">
+      <c r="C23" s="10"/>
+      <c r="D23" s="12"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="18">
+        <v>3</v>
+      </c>
+      <c r="B24" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="C24" s="10"/>
+      <c r="D24" s="12"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>4</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="C25" s="12"/>
+      <c r="D25" s="12"/>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="18">
+        <v>5</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="12"/>
+      <c r="D26" s="12"/>
+    </row>
+    <row r="27" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="5">
+        <v>6</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="12"/>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" s="10"/>
+      <c r="D31" s="11"/>
+    </row>
+    <row r="32" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>0</v>
+      </c>
+      <c r="B32" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="C32" s="10"/>
+      <c r="D32" s="12"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>1</v>
+      </c>
+      <c r="B33" s="4"/>
+      <c r="C33" s="10"/>
+      <c r="D33" s="12"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
         <v>2</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B34" s="4"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="12"/>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="18">
+        <v>3</v>
+      </c>
+      <c r="B35" s="19"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="12"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>4</v>
+      </c>
+      <c r="B36" s="19"/>
+      <c r="C36" s="12"/>
+      <c r="D36" s="12"/>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="18">
+        <v>5</v>
+      </c>
+      <c r="B37" s="19"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="18">
+        <v>6</v>
+      </c>
+      <c r="B38" s="19"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12"/>
+    </row>
+    <row r="39" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5">
         <v>7</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C7" s="3">
+      <c r="B39" s="7"/>
+      <c r="C39" s="12"/>
+      <c r="D39" s="12"/>
+    </row>
+    <row r="40" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
+      <c r="D40" s="12"/>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
+      <c r="C41" s="12"/>
+      <c r="D41" s="12"/>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
+      <c r="D42" s="12"/>
+    </row>
+    <row r="44" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="13"/>
+    </row>
+    <row r="46" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>0</v>
+      </c>
+      <c r="B46" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C46" s="10"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>1</v>
+      </c>
+      <c r="B47" s="3"/>
+      <c r="C47" s="10"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
         <v>2</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3">
+      <c r="B48" s="3"/>
+      <c r="C48" s="10"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>3</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="10"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>4</v>
+      </c>
+      <c r="B50" s="3"/>
+      <c r="C50" s="10"/>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>5</v>
+      </c>
+      <c r="B51" s="3"/>
+      <c r="C51" s="10"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>6</v>
+      </c>
+      <c r="B52" s="3"/>
+      <c r="C52" s="10"/>
+    </row>
+    <row r="53" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="5">
+        <v>7</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="10"/>
+    </row>
+    <row r="54" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
+      <c r="B54" s="12"/>
+      <c r="C54" s="12"/>
+      <c r="D54" s="12"/>
+    </row>
+    <row r="56" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B57" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C57" s="13"/>
+    </row>
+    <row r="58" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8">
+        <v>0</v>
+      </c>
+      <c r="B58" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="C58" s="10"/>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>1</v>
+      </c>
+      <c r="B59" s="3"/>
+      <c r="C59" s="10"/>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
         <v>2</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="3">
+      <c r="B60" s="3"/>
+      <c r="C60" s="10"/>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>3</v>
+      </c>
+      <c r="B61" s="3"/>
+      <c r="C61" s="10"/>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>4</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="10"/>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>5</v>
+      </c>
+      <c r="B63" s="3"/>
+      <c r="C63" s="10"/>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>6</v>
+      </c>
+      <c r="B64" s="3"/>
+      <c r="C64" s="10"/>
+    </row>
+    <row r="65" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="5">
+        <v>7</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="10"/>
+    </row>
+    <row r="66" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
+      <c r="C66" s="12"/>
+      <c r="D66" s="12"/>
+    </row>
+    <row r="68" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A68" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B69" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C69" s="13"/>
+    </row>
+    <row r="70" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="8">
+        <v>0</v>
+      </c>
+      <c r="B70" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="C70" s="10"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>1</v>
+      </c>
+      <c r="B71" s="3"/>
+      <c r="C71" s="10"/>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
         <v>2</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>10</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10" s="3">
+      <c r="B72" s="3"/>
+      <c r="C72" s="10"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>3</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="10"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>4</v>
+      </c>
+      <c r="B74" s="3"/>
+      <c r="C74" s="10"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>5</v>
+      </c>
+      <c r="B75" s="3"/>
+      <c r="C75" s="10"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>6</v>
+      </c>
+      <c r="B76" s="3"/>
+      <c r="C76" s="10"/>
+    </row>
+    <row r="77" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="5">
+        <v>7</v>
+      </c>
+      <c r="B77" s="6"/>
+      <c r="C77" s="10"/>
+    </row>
+    <row r="78" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B81" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="5">
-        <v>11</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C11" s="6">
+      <c r="C81" s="10"/>
+      <c r="D81" s="11"/>
+    </row>
+    <row r="82" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="8">
+        <v>0</v>
+      </c>
+      <c r="B82" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C82" s="10"/>
+      <c r="D82" s="12"/>
+    </row>
+    <row r="83" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A83" s="5">
         <v>1</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="C15" s="11"/>
-      <c r="D15" s="12"/>
-    </row>
-    <row r="16" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
-        <v>0</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C16" s="11"/>
-      <c r="D16" s="13"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>1</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="11"/>
-      <c r="D17" s="13"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>2</v>
-      </c>
-      <c r="B18" s="4" t="s">
+      <c r="B83" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="13"/>
-    </row>
-    <row r="19" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5">
-        <v>3</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="13"/>
-    </row>
-    <row r="20" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="1:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="32.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="B23" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D23" s="14"/>
-    </row>
-    <row r="24" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="11"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="11"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="11"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="3"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="11"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="11"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="3"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="11"/>
-    </row>
-    <row r="30" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="11"/>
-    </row>
-    <row r="31" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="C83" s="12"/>
+      <c r="D83" s="12"/>
+    </row>
+    <row r="84" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>